<commit_message>
Se Logro hacer la implementación completa de los requisitos : -REGISTRAR USUARIO -ELIMINAR USUARIO -VER PLANILLA EXCEL FALTAN: -REGISTRAR PEDIDO(PARA ESTO TOCA CONECTAR A VISTA CON MODELO PARA GENERAR UNA LISTA DE PRODUCTOS) -ELIMINAR PEDIDO -OBTENER NOMBRE ID POR NOMBRE DE USUARIO
</commit_message>
<xml_diff>
--- a/Base_Datos.xlsx
+++ b/Base_Datos.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,54 @@
       </c>
       <c r="E3" t="n">
         <v>3212156231</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rostin</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>rostin@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Guarne</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>31245456</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cristian Franco</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>cristianraigosa@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3006487895</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>